<commit_message>
Added Graphs and Ray trace for Real lenses
</commit_message>
<xml_diff>
--- a/Basicapp start/Basicapp start/RayTrace.xlsx
+++ b/Basicapp start/Basicapp start/RayTrace.xlsx
@@ -435,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AJ7" sqref="AJ7"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AL6" sqref="AL6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,10 +694,10 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <v>17.5</v>
+        <v>1000000000</v>
       </c>
       <c r="N3">
-        <v>1000000000</v>
+        <v>-17.5</v>
       </c>
       <c r="O3">
         <v>1.4338492788199999</v>
@@ -774,7 +774,7 @@
         <v>-1.7288403958263001E-2</v>
       </c>
       <c r="AO3">
-        <v>7.52</v>
+        <v>8.9700000000000006</v>
       </c>
       <c r="AP3" t="s">
         <v>14</v>

</xml_diff>